<commit_message>
9 - Completando tabela de gerenciamento de equipe com todas as etapas
</commit_message>
<xml_diff>
--- a/docs/2/tabela-gerenciamento-equipe.xlsx
+++ b/docs/2/tabela-gerenciamento-equipe.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Etapa</t>
   </si>
@@ -68,29 +68,36 @@
   </si>
   <si>
     <t>Adeilton, Carlos,Gustavo Luiz e Pedro</t>
-  </si>
-  <si>
-    <t>Programação de Funcionalidades</t>
-  </si>
-  <si>
-    <t>16/092023</t>
-  </si>
-  <si>
-    <t>Gustavo Henrique</t>
-  </si>
-  <si>
-    <t>Planos de Testes de Funcionalidades e Usabilidade</t>
-  </si>
-  <si>
-    <t>Carlos Vasconcelos</t>
-  </si>
-  <si>
-    <t>Registros de Testes de Funcionalidades  e Usabilidade</t>
   </si>
   <si>
     <t>Criar tabelas, gráficos ou dashboards com no mínimo 5 
 indicadores de desempenho 
 e metas para o processo de negócio</t>
+  </si>
+  <si>
+    <t>2º, 3º, 4º Etapa</t>
+  </si>
+  <si>
+    <t>Programação de Funcionalidades</t>
+  </si>
+  <si>
+    <t>Planos de Testes de Funcionalidades e Usabilidade</t>
+  </si>
+  <si>
+    <t>Registros de Testes de Funcionalidades  e Usabilidade</t>
+  </si>
+  <si>
+    <t>5º Etapa</t>
+  </si>
+  <si>
+    <t>Considerações Finais</t>
+  </si>
+  <si>
+    <t>Entrega de Vídeo de Apresentação Final e PDF usado na 
+Apresentação</t>
+  </si>
+  <si>
+    <t>Realização da Apresentação Final</t>
   </si>
 </sst>
 </file>
@@ -160,8 +167,8 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,80 +496,107 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4">
+        <v>45189.0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45193.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="5">
-        <v>45193.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="4">
+        <v>45166.0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>45188.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>45249.0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>45249.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="5">
-        <v>45181.0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>45185.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="3" t="s">
+    </row>
+    <row r="10">
+      <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="5">
-        <v>45181.0</v>
-      </c>
-      <c r="F9" s="5">
-        <v>45185.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="4">
-        <v>45189.0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>45193.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="D11" s="4">
+        <v>45250.0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>45250.0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>45264.0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>45264.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="20">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A2:A3"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A4:A10"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D4:D10"/>
-    <mergeCell ref="G4:G10"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="E11:E13"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>